<commit_message>
Force rename case change: Gift_ecommerce
</commit_message>
<xml_diff>
--- a/media/user_activity.xlsx
+++ b/media/user_activity.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -761,6 +761,23 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-06-15 22:17:14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix: filter by category only; add-to-cart AJAX setup
</commit_message>
<xml_diff>
--- a/media/user_activity.xlsx
+++ b/media/user_activity.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -778,6 +778,23 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-06-16 18:56:52</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated product names for bottles, notebooks, and t-shirts
</commit_message>
<xml_diff>
--- a/media/user_activity.xlsx
+++ b/media/user_activity.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -795,6 +795,74 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-06-16 23:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-06-17 08:40:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>6377384840vk@gmail.com</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-06-17 11:35:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-06-17 17:10:13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update views, models, and migrations for order tracking and dashboard enhancements
</commit_message>
<xml_diff>
--- a/media/user_activity.xlsx
+++ b/media/user_activity.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -863,6 +863,40 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:53:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-06-18 11:21:42</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix 'Continue Shopping' button redirecting to login page
</commit_message>
<xml_diff>
--- a/media/user_activity.xlsx
+++ b/media/user_activity.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -897,6 +897,23 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-06-20 17:09:08</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented onboarding flow, unique code redemption, checkout, summary and OTP login
</commit_message>
<xml_diff>
--- a/media/user_activity.xlsx
+++ b/media/user_activity.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -914,6 +914,142 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Logout</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-07-02 14:21:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2025-07-04 09:28:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2025-07-04 11:47:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2025-07-04 12:03:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Logout</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2025-07-04 12:07:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-07-04 12:08:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Logout</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-07-04 12:50:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2025-07-04 12:51:19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added created_at field to Order model and fixed reverse URL issues
</commit_message>
<xml_diff>
--- a/media/user_activity.xlsx
+++ b/media/user_activity.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1050,6 +1050,57 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Logout</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-07-04 15:44:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-07-04 15:45:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>vaishali.kh2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Logout</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-07-04 15:49:27</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>